<commit_message>
FTF and MTTC changes
</commit_message>
<xml_diff>
--- a/svmx/test_lab/test_cases/analytics/an_excleData/MTTC_data.xlsx
+++ b/svmx/test_lab/test_cases/analytics/an_excleData/MTTC_data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="54">
   <si>
     <t>Account</t>
   </si>
@@ -77,9 +77,6 @@
     <t>ScheduledDate</t>
   </si>
   <si>
-    <t>a0Nq0000003PBZS</t>
-  </si>
-  <si>
     <t>Closed</t>
   </si>
   <si>
@@ -168,6 +165,30 @@
   </si>
   <si>
     <t>a1Oq0000000KAFxEAO</t>
+  </si>
+  <si>
+    <t>closedon</t>
+  </si>
+  <si>
+    <t>Site</t>
+  </si>
+  <si>
+    <t>a1Zq0000001jyS9</t>
+  </si>
+  <si>
+    <t>2017-09-21 10:00:00</t>
+  </si>
+  <si>
+    <t>2017-09-21 13:00:00</t>
+  </si>
+  <si>
+    <t>WDStartDate1</t>
+  </si>
+  <si>
+    <t>WDEndDate1</t>
+  </si>
+  <si>
+    <t>a0Nq0000003PK1qEAG</t>
   </si>
 </sst>
 </file>
@@ -229,7 +250,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -265,8 +286,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -289,8 +316,14 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="41">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -308,6 +341,9 @@
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -325,6 +361,9 @@
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -600,14 +639,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T6"/>
+  <dimension ref="A1:Y6"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="3" max="3" width="38.83203125" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
     <col min="7" max="7" width="38" customWidth="1"/>
     <col min="11" max="11" width="22.33203125" customWidth="1"/>
@@ -616,9 +656,11 @@
     <col min="14" max="14" width="11.5" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="23.83203125" customWidth="1"/>
     <col min="20" max="20" width="24.33203125" customWidth="1"/>
+    <col min="23" max="23" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="19.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -635,7 +677,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
@@ -650,7 +692,7 @@
         <v>8</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>9</v>
@@ -674,48 +716,63 @@
         <v>15</v>
       </c>
       <c r="S1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>44</v>
+      <c r="U1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="X1" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y1" s="8" t="s">
+        <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="128" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" ht="128" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="M2" s="7">
         <v>43020.416666666664</v>
@@ -724,10 +781,10 @@
         <v>43020.458333333336</v>
       </c>
       <c r="O2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="Q2" s="1">
         <v>30</v>
@@ -736,24 +793,39 @@
         <v>42999</v>
       </c>
       <c r="S2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W2" s="4">
+        <v>42999</v>
+      </c>
+      <c r="X2" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y2" s="9" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="112" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" ht="112" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -762,10 +834,10 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -774,9 +846,9 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
     </row>
-    <row r="4" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -796,36 +868,36 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
     </row>
-    <row r="5" spans="1:20" ht="112" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" ht="112" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M5" s="5">
         <v>43020.416666666664</v>
@@ -838,7 +910,7 @@
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
     </row>
-    <row r="6" spans="1:20" ht="128" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" ht="128" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -849,7 +921,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>

</xml_diff>